<commit_message>
Push Anh Hoan Push
</commit_message>
<xml_diff>
--- a/DoAnCuoiKy/DoAnCuoiKy/bin/Debug/DuLieu.xlsx
+++ b/DoAnCuoiKy/DoAnCuoiKy/bin/Debug/DuLieu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b2h16\OneDrive\Máy tính\TeamExcrice\DoAnCuoiKy\DoAnCuoiKy\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D07539D-EF1D-46E2-A7E2-F144A70900A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DA49E96-373B-4203-A6E7-1DD96179D9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2436" yWindow="1692" windowWidth="17280" windowHeight="8880" tabRatio="662" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="80">
   <si>
     <t>Ngân hàng</t>
   </si>
@@ -261,6 +261,12 @@
   </si>
   <si>
     <t>Không có tài xế</t>
+  </si>
+  <si>
+    <t>Dream2018</t>
+  </si>
+  <si>
+    <t>47-U1</t>
   </si>
 </sst>
 </file>
@@ -667,7 +673,7 @@
         <v>123</v>
       </c>
       <c r="B3">
-        <v>170230000</v>
+        <v>360420000</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -683,7 +689,7 @@
         <v>125</v>
       </c>
       <c r="B5">
-        <v>31200000</v>
+        <v>43870000</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -739,7 +745,7 @@
         <v>132</v>
       </c>
       <c r="B12">
-        <v>8640000</v>
+        <v>7970000</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1151,16 +1157,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
@@ -1696,6 +1702,53 @@
         <v>10</v>
       </c>
       <c r="O12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13">
+        <v>123</v>
+      </c>
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="7">
+        <v>45265</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13">
+        <v>1000000</v>
+      </c>
+      <c r="H13">
+        <v>100000</v>
+      </c>
+      <c r="I13">
+        <v>100000</v>
+      </c>
+      <c r="J13">
+        <v>100000</v>
+      </c>
+      <c r="K13">
+        <v>100000</v>
+      </c>
+      <c r="L13">
+        <v>100000</v>
+      </c>
+      <c r="M13">
+        <v>100000</v>
+      </c>
+      <c r="N13" t="s">
+        <v>79</v>
+      </c>
+      <c r="O13" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>